<commit_message>
fixing readme and gantt
</commit_message>
<xml_diff>
--- a/Business Diagrams/Gantt Chart Hotel Plaza.xlsx
+++ b/Business Diagrams/Gantt Chart Hotel Plaza.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFAEF18E-87B4-4F13-99EC-B74E4839AB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C4369A-4736-4B29-B775-94BC3A91ED04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="415" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>ABOUT THIS GANTT CHART</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>SOURCE CODE DEVELOPMENT</t>
+  </si>
+  <si>
+    <t>"Item" Class</t>
   </si>
   <si>
     <t>"Guest" Class</t>
@@ -1671,8 +1674,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:G40" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B9:G40" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DD82988E-1813-40AE-BDE7-9F0200A703CB}" name="Milestones4352" displayName="Milestones4352" ref="B9:G41" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="B9:G41" xr:uid="{29E5A880-80D5-4B65-B5FB-8FB3913D3D27}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -2133,10 +2136,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BP42"/>
+  <dimension ref="A1:BP43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A32" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5824,7 +5827,7 @@
         <v/>
       </c>
       <c r="AN22" s="17" t="str">
-        <f t="shared" ref="AN22:BC39" ca="1" si="9">IF(AND($C22="Goal",AN$7&gt;=$F22,AN$7&lt;=$F22+$G22-1),2,IF(AND($C22="Milestone",AN$7&gt;=$F22,AN$7&lt;=$F22+$G22-1),1,""))</f>
+        <f t="shared" ref="AN22:BC40" ca="1" si="9">IF(AND($C22="Goal",AN$7&gt;=$F22,AN$7&lt;=$F22+$G22-1),2,IF(AND($C22="Milestone",AN$7&gt;=$F22,AN$7&lt;=$F22+$G22-1),1,""))</f>
         <v/>
       </c>
       <c r="AO22" s="17" t="str">
@@ -5888,7 +5891,7 @@
         <v/>
       </c>
       <c r="BD22" s="17" t="str">
-        <f t="shared" ref="BD22:BL39" ca="1" si="10">IF(AND($C22="Goal",BD$7&gt;=$F22,BD$7&lt;=$F22+$G22-1),2,IF(AND($C22="Milestone",BD$7&gt;=$F22,BD$7&lt;=$F22+$G22-1),1,""))</f>
+        <f t="shared" ref="BD22:BL40" ca="1" si="10">IF(AND($C22="Goal",BD$7&gt;=$F22,BD$7&lt;=$F22+$G22-1),2,IF(AND($C22="Milestone",BD$7&gt;=$F22,BD$7&lt;=$F22+$G22-1),1,""))</f>
         <v/>
       </c>
       <c r="BE22" s="17" t="str">
@@ -6010,7 +6013,7 @@
         <v/>
       </c>
       <c r="Y23" s="17" t="str">
-        <f t="shared" ref="Y23:AM39" ca="1" si="11">IF(AND($C23="Goal",Y$7&gt;=$F23,Y$7&lt;=$F23+$G23-1),2,IF(AND($C23="Milestone",Y$7&gt;=$F23,Y$7&lt;=$F23+$G23-1),1,""))</f>
+        <f t="shared" ref="Y23:AM40" ca="1" si="11">IF(AND($C23="Goal",Y$7&gt;=$F23,Y$7&lt;=$F23+$G23-1),2,IF(AND($C23="Milestone",Y$7&gt;=$F23,Y$7&lt;=$F23+$G23-1),1,""))</f>
         <v/>
       </c>
       <c r="Z23" s="17" t="str">
@@ -6506,7 +6509,7 @@
         <v>41</v>
       </c>
       <c r="E26" s="21">
-        <v>0.65</v>
+        <v>1</v>
       </c>
       <c r="F26" s="22">
         <v>44520</v>
@@ -6584,7 +6587,7 @@
       <c r="G27" s="23"/>
       <c r="H27" s="20"/>
       <c r="I27" s="17" t="str">
-        <f t="shared" ref="I27:X39" ca="1" si="12">IF(AND($C27="Goal",I$7&gt;=$F27,I$7&lt;=$F27+$G27-1),2,IF(AND($C27="Milestone",I$7&gt;=$F27,I$7&lt;=$F27+$G27-1),1,""))</f>
+        <f t="shared" ref="I27:X40" ca="1" si="12">IF(AND($C27="Goal",I$7&gt;=$F27,I$7&lt;=$F27+$G27-1),2,IF(AND($C27="Milestone",I$7&gt;=$F27,I$7&lt;=$F27+$G27-1),1,""))</f>
         <v/>
       </c>
       <c r="J27" s="17" t="str">
@@ -6826,233 +6829,65 @@
         <v>44520</v>
       </c>
       <c r="G28" s="23">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H28" s="20"/>
-      <c r="I28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="J28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="K28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="L28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="M28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="N28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="O28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="P28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="Q28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="R28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="S28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="T28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="U28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="V28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="W28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="X28" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="Y28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="Z28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AA28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AB28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AC28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AD28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AE28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AF28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AG28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AH28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AI28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AJ28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AK28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AL28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AM28" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AN28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AO28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AP28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AQ28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AR28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AS28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AT28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AU28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AV28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AW28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AX28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AY28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AZ28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BA28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BB28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BC28" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BD28" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BE28" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BF28" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BG28" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BH28" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BI28" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BJ28" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BK28" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BL28" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="17"/>
+      <c r="U28" s="17"/>
+      <c r="V28" s="17"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="17"/>
+      <c r="AA28" s="17"/>
+      <c r="AB28" s="17"/>
+      <c r="AC28" s="17"/>
+      <c r="AD28" s="17"/>
+      <c r="AE28" s="17"/>
+      <c r="AF28" s="17"/>
+      <c r="AG28" s="17"/>
+      <c r="AH28" s="17"/>
+      <c r="AI28" s="17"/>
+      <c r="AJ28" s="17"/>
+      <c r="AK28" s="17"/>
+      <c r="AL28" s="17"/>
+      <c r="AM28" s="17"/>
+      <c r="AN28" s="17"/>
+      <c r="AO28" s="17"/>
+      <c r="AP28" s="17"/>
+      <c r="AQ28" s="17"/>
+      <c r="AR28" s="17"/>
+      <c r="AS28" s="17"/>
+      <c r="AT28" s="17"/>
+      <c r="AU28" s="17"/>
+      <c r="AV28" s="17"/>
+      <c r="AW28" s="17"/>
+      <c r="AX28" s="17"/>
+      <c r="AY28" s="17"/>
+      <c r="AZ28" s="17"/>
+      <c r="BA28" s="17"/>
+      <c r="BB28" s="17"/>
+      <c r="BC28" s="17"/>
+      <c r="BD28" s="17"/>
+      <c r="BE28" s="17"/>
+      <c r="BF28" s="17"/>
+      <c r="BG28" s="17"/>
+      <c r="BH28" s="17"/>
+      <c r="BI28" s="17"/>
+      <c r="BJ28" s="17"/>
+      <c r="BK28" s="17"/>
+      <c r="BL28" s="17"/>
     </row>
     <row r="29" spans="1:64" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
@@ -7309,7 +7144,7 @@
         <v>40</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E30" s="21">
         <v>1</v>
@@ -7810,65 +7645,233 @@
         <v>44520</v>
       </c>
       <c r="G32" s="23">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H32" s="20"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="17"/>
-      <c r="O32" s="17"/>
-      <c r="P32" s="17"/>
-      <c r="Q32" s="17"/>
-      <c r="R32" s="17"/>
-      <c r="S32" s="17"/>
-      <c r="T32" s="17"/>
-      <c r="U32" s="17"/>
-      <c r="V32" s="17"/>
-      <c r="W32" s="17"/>
-      <c r="X32" s="17"/>
-      <c r="Y32" s="17"/>
-      <c r="Z32" s="17"/>
-      <c r="AA32" s="17"/>
-      <c r="AB32" s="17"/>
-      <c r="AC32" s="17"/>
-      <c r="AD32" s="17"/>
-      <c r="AE32" s="17"/>
-      <c r="AF32" s="17"/>
-      <c r="AG32" s="17"/>
-      <c r="AH32" s="17"/>
-      <c r="AI32" s="17"/>
-      <c r="AJ32" s="17"/>
-      <c r="AK32" s="17"/>
-      <c r="AL32" s="17"/>
-      <c r="AM32" s="17"/>
-      <c r="AN32" s="17"/>
-      <c r="AO32" s="17"/>
-      <c r="AP32" s="17"/>
-      <c r="AQ32" s="17"/>
-      <c r="AR32" s="17"/>
-      <c r="AS32" s="17"/>
-      <c r="AT32" s="17"/>
-      <c r="AU32" s="17"/>
-      <c r="AV32" s="17"/>
-      <c r="AW32" s="17"/>
-      <c r="AX32" s="17"/>
-      <c r="AY32" s="17"/>
-      <c r="AZ32" s="17"/>
-      <c r="BA32" s="17"/>
-      <c r="BB32" s="17"/>
-      <c r="BC32" s="17"/>
-      <c r="BD32" s="17"/>
-      <c r="BE32" s="17"/>
-      <c r="BF32" s="17"/>
-      <c r="BG32" s="17"/>
-      <c r="BH32" s="17"/>
-      <c r="BI32" s="17"/>
-      <c r="BJ32" s="17"/>
-      <c r="BK32" s="17"/>
-      <c r="BL32" s="17"/>
+      <c r="I32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="J32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="K32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="L32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="M32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="N32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="O32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="P32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="Q32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="R32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="S32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="T32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="U32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="V32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="W32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="X32" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="Y32" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="Z32" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AA32" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AB32" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AC32" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AD32" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AE32" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AF32" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AG32" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AH32" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AI32" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AJ32" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AK32" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AL32" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AM32" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AN32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AO32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AP32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AQ32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AR32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AS32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AT32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AU32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AV32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AW32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AX32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AY32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AZ32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BA32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BB32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BC32" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BD32" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BE32" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BF32" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BG32" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BH32" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BI32" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BJ32" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BK32" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BL32" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
     </row>
     <row r="33" spans="1:65" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
@@ -7888,7 +7891,7 @@
         <v>44520</v>
       </c>
       <c r="G33" s="23">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H33" s="20"/>
       <c r="I33" s="17"/>
@@ -7957,7 +7960,7 @@
         <v>40</v>
       </c>
       <c r="D34" s="20" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="E34" s="21">
         <v>1</v>
@@ -7966,233 +7969,65 @@
         <v>44520</v>
       </c>
       <c r="G34" s="23">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H34" s="20"/>
-      <c r="I34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="J34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="K34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="L34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="M34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="N34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="O34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="P34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="Q34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="R34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="S34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="T34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="U34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="V34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="W34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="X34" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="Y34" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="Z34" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AA34" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AB34" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AC34" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AD34" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AE34" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AF34" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AG34" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AH34" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AI34" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AJ34" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AK34" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AL34" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AM34" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AN34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AO34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AP34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AQ34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AR34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AS34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AT34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AU34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AV34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AW34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AX34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AY34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AZ34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BA34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BB34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BC34" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BD34" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BE34" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BF34" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BG34" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BH34" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BI34" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BJ34" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BK34" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BL34" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+      <c r="W34" s="17"/>
+      <c r="X34" s="17"/>
+      <c r="Y34" s="17"/>
+      <c r="Z34" s="17"/>
+      <c r="AA34" s="17"/>
+      <c r="AB34" s="17"/>
+      <c r="AC34" s="17"/>
+      <c r="AD34" s="17"/>
+      <c r="AE34" s="17"/>
+      <c r="AF34" s="17"/>
+      <c r="AG34" s="17"/>
+      <c r="AH34" s="17"/>
+      <c r="AI34" s="17"/>
+      <c r="AJ34" s="17"/>
+      <c r="AK34" s="17"/>
+      <c r="AL34" s="17"/>
+      <c r="AM34" s="17"/>
+      <c r="AN34" s="17"/>
+      <c r="AO34" s="17"/>
+      <c r="AP34" s="17"/>
+      <c r="AQ34" s="17"/>
+      <c r="AR34" s="17"/>
+      <c r="AS34" s="17"/>
+      <c r="AT34" s="17"/>
+      <c r="AU34" s="17"/>
+      <c r="AV34" s="17"/>
+      <c r="AW34" s="17"/>
+      <c r="AX34" s="17"/>
+      <c r="AY34" s="17"/>
+      <c r="AZ34" s="17"/>
+      <c r="BA34" s="17"/>
+      <c r="BB34" s="17"/>
+      <c r="BC34" s="17"/>
+      <c r="BD34" s="17"/>
+      <c r="BE34" s="17"/>
+      <c r="BF34" s="17"/>
+      <c r="BG34" s="17"/>
+      <c r="BH34" s="17"/>
+      <c r="BI34" s="17"/>
+      <c r="BJ34" s="17"/>
+      <c r="BK34" s="17"/>
+      <c r="BL34" s="17"/>
     </row>
     <row r="35" spans="1:65" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
@@ -8203,7 +8038,7 @@
         <v>40</v>
       </c>
       <c r="D35" s="20" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="E35" s="21">
         <v>1</v>
@@ -8215,62 +8050,230 @@
         <v>13</v>
       </c>
       <c r="H35" s="20"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="17"/>
-      <c r="N35" s="17"/>
-      <c r="O35" s="17"/>
-      <c r="P35" s="17"/>
-      <c r="Q35" s="17"/>
-      <c r="R35" s="17"/>
-      <c r="S35" s="17"/>
-      <c r="T35" s="17"/>
-      <c r="U35" s="17"/>
-      <c r="V35" s="17"/>
-      <c r="W35" s="17"/>
-      <c r="X35" s="17"/>
-      <c r="Y35" s="17"/>
-      <c r="Z35" s="17"/>
-      <c r="AA35" s="17"/>
-      <c r="AB35" s="17"/>
-      <c r="AC35" s="17"/>
-      <c r="AD35" s="17"/>
-      <c r="AE35" s="17"/>
-      <c r="AF35" s="17"/>
-      <c r="AG35" s="17"/>
-      <c r="AH35" s="17"/>
-      <c r="AI35" s="17"/>
-      <c r="AJ35" s="17"/>
-      <c r="AK35" s="17"/>
-      <c r="AL35" s="17"/>
-      <c r="AM35" s="17"/>
-      <c r="AN35" s="17"/>
-      <c r="AO35" s="17"/>
-      <c r="AP35" s="17"/>
-      <c r="AQ35" s="17"/>
-      <c r="AR35" s="17"/>
-      <c r="AS35" s="17"/>
-      <c r="AT35" s="17"/>
-      <c r="AU35" s="17"/>
-      <c r="AV35" s="17"/>
-      <c r="AW35" s="17"/>
-      <c r="AX35" s="17"/>
-      <c r="AY35" s="17"/>
-      <c r="AZ35" s="17"/>
-      <c r="BA35" s="17"/>
-      <c r="BB35" s="17"/>
-      <c r="BC35" s="17"/>
-      <c r="BD35" s="17"/>
-      <c r="BE35" s="17"/>
-      <c r="BF35" s="17"/>
-      <c r="BG35" s="17"/>
-      <c r="BH35" s="17"/>
-      <c r="BI35" s="17"/>
-      <c r="BJ35" s="17"/>
-      <c r="BK35" s="17"/>
-      <c r="BL35" s="17"/>
+      <c r="I35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="J35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="K35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="L35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="M35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="N35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="O35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="P35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="Q35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="R35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="S35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="T35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="U35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="V35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="W35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="X35" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="Y35" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="Z35" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AA35" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AB35" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AC35" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AD35" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AE35" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AF35" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AG35" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AH35" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AI35" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AJ35" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AK35" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AL35" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AM35" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AN35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AO35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AP35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AQ35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AR35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AS35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AT35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AU35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AV35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AW35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AX35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AY35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AZ35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BA35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BB35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BC35" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BD35" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BE35" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BF35" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BG35" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BH35" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BI35" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BJ35" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BK35" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BL35" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
     </row>
     <row r="36" spans="1:65" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="9"/>
@@ -8281,7 +8284,7 @@
         <v>40</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="E36" s="21">
         <v>1</v>
@@ -8352,14 +8355,24 @@
     </row>
     <row r="37" spans="1:65" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9"/>
-      <c r="B37" s="71" t="s">
+      <c r="B37" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="21"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="23"/>
+      <c r="C37" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" s="21">
+        <v>1</v>
+      </c>
+      <c r="F37" s="22">
+        <v>44520</v>
+      </c>
+      <c r="G37" s="23">
+        <v>13</v>
+      </c>
       <c r="H37" s="20"/>
       <c r="I37" s="17"/>
       <c r="J37" s="17"/>
@@ -8420,24 +8433,14 @@
     </row>
     <row r="38" spans="1:65" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9"/>
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38" s="21">
-        <v>0</v>
-      </c>
-      <c r="F38" s="22">
-        <v>44533</v>
-      </c>
-      <c r="G38" s="23">
-        <v>2</v>
-      </c>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="23"/>
       <c r="H38" s="20"/>
       <c r="I38" s="17"/>
       <c r="J38" s="17"/>
@@ -8505,10 +8508,10 @@
         <v>27</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="E39" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39" s="22">
         <v>44533</v>
@@ -8517,307 +8520,385 @@
         <v>2</v>
       </c>
       <c r="H39" s="20"/>
-      <c r="I39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="J39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="K39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="L39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="M39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="N39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="O39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="P39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="Q39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="R39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="S39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="T39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="U39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="V39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="W39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="X39" s="17" t="str">
-        <f t="shared" ca="1" si="12"/>
-        <v/>
-      </c>
-      <c r="Y39" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="Z39" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AA39" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AB39" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AC39" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AD39" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AE39" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AF39" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AG39" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AH39" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AI39" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AJ39" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AK39" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AL39" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AM39" s="17" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v/>
-      </c>
-      <c r="AN39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AO39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AP39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AQ39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AR39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AS39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AT39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AU39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AV39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AW39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AX39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AY39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="AZ39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BA39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BB39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BC39" s="17" t="str">
-        <f t="shared" ca="1" si="9"/>
-        <v/>
-      </c>
-      <c r="BD39" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BE39" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BF39" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BG39" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BH39" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BI39" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BJ39" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BK39" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BL39" s="17" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v/>
-      </c>
-      <c r="BM39" s="46"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="17"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="17"/>
+      <c r="T39" s="17"/>
+      <c r="U39" s="17"/>
+      <c r="V39" s="17"/>
+      <c r="W39" s="17"/>
+      <c r="X39" s="17"/>
+      <c r="Y39" s="17"/>
+      <c r="Z39" s="17"/>
+      <c r="AA39" s="17"/>
+      <c r="AB39" s="17"/>
+      <c r="AC39" s="17"/>
+      <c r="AD39" s="17"/>
+      <c r="AE39" s="17"/>
+      <c r="AF39" s="17"/>
+      <c r="AG39" s="17"/>
+      <c r="AH39" s="17"/>
+      <c r="AI39" s="17"/>
+      <c r="AJ39" s="17"/>
+      <c r="AK39" s="17"/>
+      <c r="AL39" s="17"/>
+      <c r="AM39" s="17"/>
+      <c r="AN39" s="17"/>
+      <c r="AO39" s="17"/>
+      <c r="AP39" s="17"/>
+      <c r="AQ39" s="17"/>
+      <c r="AR39" s="17"/>
+      <c r="AS39" s="17"/>
+      <c r="AT39" s="17"/>
+      <c r="AU39" s="17"/>
+      <c r="AV39" s="17"/>
+      <c r="AW39" s="17"/>
+      <c r="AX39" s="17"/>
+      <c r="AY39" s="17"/>
+      <c r="AZ39" s="17"/>
+      <c r="BA39" s="17"/>
+      <c r="BB39" s="17"/>
+      <c r="BC39" s="17"/>
+      <c r="BD39" s="17"/>
+      <c r="BE39" s="17"/>
+      <c r="BF39" s="17"/>
+      <c r="BG39" s="17"/>
+      <c r="BH39" s="17"/>
+      <c r="BI39" s="17"/>
+      <c r="BJ39" s="17"/>
+      <c r="BK39" s="17"/>
+      <c r="BL39" s="17"/>
     </row>
     <row r="40" spans="1:65" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="10"/>
-      <c r="B40" s="70" t="s">
+      <c r="A40" s="9"/>
+      <c r="B40" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="32"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="43"/>
+      <c r="C40" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="21">
+        <v>1</v>
+      </c>
+      <c r="F40" s="22">
+        <v>44533</v>
+      </c>
+      <c r="G40" s="23">
+        <v>2</v>
+      </c>
       <c r="H40" s="20"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
-      <c r="K40" s="44"/>
-      <c r="L40" s="44"/>
-      <c r="M40" s="44"/>
-      <c r="N40" s="44"/>
-      <c r="O40" s="44"/>
-      <c r="P40" s="44"/>
-      <c r="Q40" s="44"/>
-      <c r="R40" s="44"/>
-      <c r="S40" s="44"/>
-      <c r="T40" s="44"/>
-      <c r="U40" s="44"/>
-      <c r="V40" s="44"/>
-      <c r="W40" s="44"/>
-      <c r="X40" s="44"/>
-      <c r="Y40" s="44"/>
-      <c r="Z40" s="44"/>
-      <c r="AA40" s="44"/>
-      <c r="AB40" s="44"/>
-      <c r="AC40" s="44"/>
-      <c r="AD40" s="44"/>
-      <c r="AE40" s="44"/>
-      <c r="AF40" s="44"/>
-      <c r="AG40" s="44"/>
-      <c r="AH40" s="44"/>
-      <c r="AI40" s="44"/>
-      <c r="AJ40" s="44"/>
-      <c r="AK40" s="44"/>
-      <c r="AL40" s="44"/>
-      <c r="AM40" s="44"/>
-      <c r="AN40" s="44"/>
-      <c r="AO40" s="44"/>
-      <c r="AP40" s="44"/>
-      <c r="AQ40" s="44"/>
-      <c r="AR40" s="44"/>
-      <c r="AS40" s="44"/>
-      <c r="AT40" s="44"/>
-      <c r="AU40" s="44"/>
-      <c r="AV40" s="44"/>
-      <c r="AW40" s="44"/>
-      <c r="AX40" s="44"/>
-      <c r="AY40" s="44"/>
-      <c r="AZ40" s="44"/>
-      <c r="BA40" s="44"/>
-      <c r="BB40" s="44"/>
-      <c r="BC40" s="44"/>
-      <c r="BD40" s="44"/>
-      <c r="BE40" s="44"/>
-      <c r="BF40" s="44"/>
-      <c r="BG40" s="44"/>
-      <c r="BH40" s="44"/>
-      <c r="BI40" s="44"/>
-      <c r="BJ40" s="44"/>
-      <c r="BK40" s="44"/>
-      <c r="BL40" s="44"/>
+      <c r="I40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="J40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="K40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="L40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="M40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="N40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="O40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="P40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="Q40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="R40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="S40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="T40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="U40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="V40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="W40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="X40" s="17" t="str">
+        <f t="shared" ca="1" si="12"/>
+        <v/>
+      </c>
+      <c r="Y40" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="Z40" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AA40" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AB40" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AC40" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AD40" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AE40" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AF40" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AG40" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AH40" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AI40" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AJ40" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AK40" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AL40" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AM40" s="17" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v/>
+      </c>
+      <c r="AN40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AO40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AP40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AQ40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AR40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AS40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AT40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AU40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AV40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AW40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AX40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AY40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="AZ40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BA40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BB40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BC40" s="17" t="str">
+        <f t="shared" ca="1" si="9"/>
+        <v/>
+      </c>
+      <c r="BD40" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BE40" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BF40" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BG40" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BH40" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BI40" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BJ40" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BK40" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BL40" s="17" t="str">
+        <f t="shared" ca="1" si="10"/>
+        <v/>
+      </c>
+      <c r="BM40" s="46"/>
     </row>
-    <row r="41" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D41" s="4"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="3"/>
+    <row r="41" spans="1:65" s="1" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="10"/>
+      <c r="B41" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="44"/>
+      <c r="J41" s="44"/>
+      <c r="K41" s="44"/>
+      <c r="L41" s="44"/>
+      <c r="M41" s="44"/>
+      <c r="N41" s="44"/>
+      <c r="O41" s="44"/>
+      <c r="P41" s="44"/>
+      <c r="Q41" s="44"/>
+      <c r="R41" s="44"/>
+      <c r="S41" s="44"/>
+      <c r="T41" s="44"/>
+      <c r="U41" s="44"/>
+      <c r="V41" s="44"/>
+      <c r="W41" s="44"/>
+      <c r="X41" s="44"/>
+      <c r="Y41" s="44"/>
+      <c r="Z41" s="44"/>
+      <c r="AA41" s="44"/>
+      <c r="AB41" s="44"/>
+      <c r="AC41" s="44"/>
+      <c r="AD41" s="44"/>
+      <c r="AE41" s="44"/>
+      <c r="AF41" s="44"/>
+      <c r="AG41" s="44"/>
+      <c r="AH41" s="44"/>
+      <c r="AI41" s="44"/>
+      <c r="AJ41" s="44"/>
+      <c r="AK41" s="44"/>
+      <c r="AL41" s="44"/>
+      <c r="AM41" s="44"/>
+      <c r="AN41" s="44"/>
+      <c r="AO41" s="44"/>
+      <c r="AP41" s="44"/>
+      <c r="AQ41" s="44"/>
+      <c r="AR41" s="44"/>
+      <c r="AS41" s="44"/>
+      <c r="AT41" s="44"/>
+      <c r="AU41" s="44"/>
+      <c r="AV41" s="44"/>
+      <c r="AW41" s="44"/>
+      <c r="AX41" s="44"/>
+      <c r="AY41" s="44"/>
+      <c r="AZ41" s="44"/>
+      <c r="BA41" s="44"/>
+      <c r="BB41" s="44"/>
+      <c r="BC41" s="44"/>
+      <c r="BD41" s="44"/>
+      <c r="BE41" s="44"/>
+      <c r="BF41" s="44"/>
+      <c r="BG41" s="44"/>
+      <c r="BH41" s="44"/>
+      <c r="BI41" s="44"/>
+      <c r="BJ41" s="44"/>
+      <c r="BK41" s="44"/>
+      <c r="BL41" s="44"/>
     </row>
     <row r="42" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D42" s="5"/>
+      <c r="D42" s="4"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="1:65" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D43" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -8830,7 +8911,7 @@
     <mergeCell ref="N4:Q4"/>
     <mergeCell ref="S4:V4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E9:E40">
+  <conditionalFormatting sqref="E9:E41">
     <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -8844,7 +8925,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL40">
+  <conditionalFormatting sqref="I7:BL41">
     <cfRule type="expression" dxfId="21" priority="1">
       <formula>AND(TODAY()&gt;=I$7,TODAY()&lt;J$7)</formula>
     </cfRule>
@@ -8864,7 +8945,7 @@
       <formula>AND(I$7&lt;=EOMONTH($I$7,1),I$7&gt;EOMONTH($I$7,0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10:BL39">
+  <conditionalFormatting sqref="I10:BL40">
     <cfRule type="expression" dxfId="17" priority="7" stopIfTrue="1">
       <formula>AND($C10="Low Risk",I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
@@ -8881,7 +8962,7 @@
       <formula>AND(LEN($C10)=0,I$7&gt;=$F10,I$7&lt;=$F10+$G10-1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I40:BL40">
+  <conditionalFormatting sqref="I41:BL41">
     <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",I$7&gt;=#REF!,I$7&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
@@ -8902,7 +8983,7 @@
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Scrolling Increment" prompt="Changing this number will scroll the Gantt Chart view." sqref="C7" xr:uid="{662A47A0-7258-440E-8D71-BC54CBC9C651}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C39" xr:uid="{12A8278F-D51D-4B98-A311-DB5FCD18D214}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C12:C40" xr:uid="{12A8278F-D51D-4B98-A311-DB5FCD18D214}">
       <formula1>"Goal,Milestone,On Track, Low Risk, Med Risk, High Risk"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="C11" xr:uid="{218D9212-09C8-4DA2-9014-64503951B170}">
@@ -8916,8 +8997,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="A scrollbar is in cells I8 through BL8. _x000a_To jump forward or backward in the timeline, enter a value of 0 or higher in cell C7._x000a_A value of 0 takes you to the beginning of the chart." sqref="A8" xr:uid="{737D7247-B514-41B2-94CC-2F538E17DE66}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row contains headers for the project schedule.  B9 through G9 contains schedule information.  Cells I9 through BL9 contain the first letter of each day of the week for the date above that heading._x000a_All project timeline charting is auto generated." sqref="A9" xr:uid="{6AB925DC-9BC9-4EC3-A848-25121289EECD}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Project information starting in cell B11 through cell G11. _x000a_Enter Milestone Description, select a Category, assign someone to the task, and enter the progress, start date, and number of days for the task to start charting._x000a_" sqref="A11" xr:uid="{77315CCB-C571-42B0-8983-9C17BB04F75F}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Gantt milestone data. DO NOT enter anything in this row. _x000a_To add more items, insert new rows above this one._x000a_" sqref="A40" xr:uid="{659FD5CB-B62B-4854-B8A9-29F1F70930AC}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is an empty row" sqref="A39" xr:uid="{60F6BB2A-523D-41BA-B324-85E19FB9FF7E}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This row marks the end of the Gantt milestone data. DO NOT enter anything in this row. _x000a_To add more items, insert new rows above this one._x000a_" sqref="A41" xr:uid="{659FD5CB-B62B-4854-B8A9-29F1F70930AC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is an empty row" sqref="A40" xr:uid="{60F6BB2A-523D-41BA-B324-85E19FB9FF7E}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -8974,7 +9055,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E9:E40</xm:sqref>
+          <xm:sqref>E9:E41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="12" id="{A1EFF969-3CBB-4DB2-A4C9-47B01FE32C86}">
@@ -8993,7 +9074,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I40:BL40</xm:sqref>
+          <xm:sqref>I41:BL41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="92" id="{39412BF5-D1E8-4731-95F6-6B0C252D35F8}">
@@ -9012,7 +9093,7 @@
               <x14:cfIcon iconSet="3Signs" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>I10:BL39</xm:sqref>
+          <xm:sqref>I10:BL40</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -9021,6 +9102,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A22D0D31444014A85663465D34FC8A3" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a6d37268c3689967fd96597fd9f98d6d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0680abb9-2b2a-45b5-abf5-037da14d9ef0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="230bd39aa74a6b43fdcc0a20f001bbb0" ns3:_="">
     <xsd:import namespace="0680abb9-2b2a-45b5-abf5-037da14d9ef0"/>
@@ -9152,22 +9248,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="0680abb9-2b2a-45b5-abf5-037da14d9ef0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9966656C-773E-41B7-AE8A-C2BED73E070D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9183,28 +9288,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AA4BA2A8-DB97-40F9-8DB6-154C09C7467C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="0680abb9-2b2a-45b5-abf5-037da14d9ef0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{39060724-9CA2-4290-8A0C-B53624A594E7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>